<commit_message>
Can advance to next level
</commit_message>
<xml_diff>
--- a/De_Ridder_Jonas_Game.xlsx
+++ b/De_Ridder_Jonas_Game.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Programming2\00_Game\De_Ridder_Jonas_Super_Paper_Mario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94F2F0C-37F0-4920-99A8-CA0692FD6942}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53959BA2-21AD-4749-89B2-BD06514539C3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Game rubric" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Camera</t>
   </si>
@@ -103,19 +103,22 @@
     <t>Animation system based on data from a file</t>
   </si>
   <si>
-    <t>Moving animation</t>
-  </si>
-  <si>
     <t>Shows player health</t>
   </si>
   <si>
     <t>Free moving camera</t>
   </si>
   <si>
-    <t>Player can be hit by enemies &amp; projectiles. Player can jump on enemies, kill enemies with Pixl</t>
-  </si>
-  <si>
-    <t>Player can move around, enemies walk around and attack</t>
+    <t>Mario moving &amp; attacking, Enemies walking</t>
+  </si>
+  <si>
+    <t>Player can be hit by enemies &amp; projectiles. Player can jump on enemies, kill enemies with Pixl. Player can pickup items</t>
+  </si>
+  <si>
+    <t>Player can move around, enemies walk around and attack, player can change attack, use items and advance to next level</t>
+  </si>
+  <si>
+    <t>Items and pixls</t>
   </si>
 </sst>
 </file>
@@ -515,11 +518,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -548,7 +551,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
@@ -556,10 +559,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
@@ -567,7 +570,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>25</v>
@@ -592,7 +595,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
@@ -623,11 +626,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -701,7 +704,10 @@
         <v>12</v>
       </c>
       <c r="B8" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fix pixl inventory visual bug
</commit_message>
<xml_diff>
--- a/De_Ridder_Jonas_Game.xlsx
+++ b/De_Ridder_Jonas_Game.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Programming2\00_Game\De_Ridder_Jonas_Super_Paper_Mario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577B8303-321C-49C3-A0FD-332F64D2BE59}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC68B69-A959-4473-84A9-AC035D627BF8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Game rubric" sheetId="2" r:id="rId1"/>
@@ -115,10 +115,10 @@
     <t>Player can be hit by enemies &amp; projectiles. Player can jump on enemies, kill enemies with Pixl. Player can pickup items</t>
   </si>
   <si>
-    <t>Player can move around, enemies walk around and attack, player can change attack, use items and advance to next level</t>
-  </si>
-  <si>
     <t>Items and pixls</t>
+  </si>
+  <si>
+    <t>Player can move around, enemies walk around and attack, player can change attack, use items, advance to next level, interact with objects</t>
   </si>
 </sst>
 </file>
@@ -518,11 +518,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,7 +559,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>24</v>
@@ -581,10 +581,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
@@ -626,7 +626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -707,7 +707,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Title screen + sound settings
</commit_message>
<xml_diff>
--- a/De_Ridder_Jonas_Game.xlsx
+++ b/De_Ridder_Jonas_Game.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Programming2\00_Game\De_Ridder_Jonas_Super_Paper_Mario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C8B5CF-EE2A-4392-9ABA-B412F4CBBBC7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46C0B2A-A511-456A-87E0-A20DF16EF3C9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Game rubric" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Camera</t>
   </si>
@@ -118,10 +118,13 @@
     <t>Player can move around, enemies walk around and attack, player can change attack, use items, advance to next level, interact with objects</t>
   </si>
   <si>
-    <t>Shows player health and coins</t>
-  </si>
-  <si>
     <t>basic particles (coins &amp; smoke when enemy dies)</t>
+  </si>
+  <si>
+    <t>Show Player info + Menu system</t>
+  </si>
+  <si>
+    <t>Background music</t>
   </si>
 </sst>
 </file>
@@ -521,7 +524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -595,10 +598,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
@@ -606,9 +609,11 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
@@ -629,7 +634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -729,7 +734,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">

</xml_diff>